<commit_message>
Arreglando barras de progreso y metas cumplidas
</commit_message>
<xml_diff>
--- a/mdrt/mdrt_actual.xlsx
+++ b/mdrt/mdrt_actual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/ ANTIGRAVITY/mdrt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA69684-24A6-8740-9FDE-FDC471AFA10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2461543D-A250-F84D-B3BF-E2209E1AC64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B49CA26D-17E4-1041-9F6C-DBD86CE9FF01}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16140" xr2:uid="{B49CA26D-17E4-1041-9F6C-DBD86CE9FF01}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -364,7 +364,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -399,13 +399,6 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -420,39 +413,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="59">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <border>
         <left style="thin">
@@ -519,670 +480,6 @@
         </top>
         <bottom style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color rgb="FF002060"/>
-        </left>
-        <right style="hair">
-          <color rgb="FF002060"/>
-        </right>
-        <top style="hair">
-          <color rgb="FF002060"/>
-        </top>
-        <bottom style="hair">
-          <color rgb="FF002060"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color rgb="FF002060"/>
-        </left>
-        <right style="hair">
-          <color rgb="FF002060"/>
-        </right>
-        <top style="hair">
-          <color rgb="FF002060"/>
-        </top>
-        <bottom style="hair">
-          <color rgb="FF002060"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color rgb="FF002060"/>
-        </left>
-        <right style="hair">
-          <color rgb="FF002060"/>
-        </right>
-        <top style="hair">
-          <color rgb="FF002060"/>
-        </top>
-        <bottom style="hair">
-          <color rgb="FF002060"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color rgb="FF002060"/>
-        </left>
-        <right style="hair">
-          <color rgb="FF002060"/>
-        </right>
-        <top style="hair">
-          <color rgb="FF002060"/>
-        </top>
-        <bottom style="hair">
-          <color rgb="FF002060"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color rgb="FF002060"/>
-        </left>
-        <right style="hair">
-          <color rgb="FF002060"/>
-        </right>
-        <top style="hair">
-          <color rgb="FF002060"/>
-        </top>
-        <bottom style="hair">
-          <color rgb="FF002060"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color rgb="FF002060"/>
-        </left>
-        <right style="hair">
-          <color rgb="FF002060"/>
-        </right>
-        <top style="hair">
-          <color rgb="FF002060"/>
-        </top>
-        <bottom style="hair">
-          <color rgb="FF002060"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color rgb="FF002060"/>
-        </left>
-        <right style="hair">
-          <color rgb="FF002060"/>
-        </right>
-        <top style="hair">
-          <color rgb="FF002060"/>
-        </top>
-        <bottom style="hair">
-          <color rgb="FF002060"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color rgb="FF002060"/>
-        </left>
-        <right style="hair">
-          <color rgb="FF002060"/>
-        </right>
-        <top style="hair">
-          <color rgb="FF002060"/>
-        </top>
-        <bottom style="hair">
-          <color rgb="FF002060"/>
         </bottom>
       </border>
     </dxf>
@@ -1596,19 +893,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E315FDF5-0096-7641-98E2-79A7C2A6467A}" name="Tabla1354" displayName="Tabla1354" ref="A1:G51" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E315FDF5-0096-7641-98E2-79A7C2A6467A}" name="Tabla1354" displayName="Tabla1354" ref="A1:G51" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:G51" xr:uid="{E315FDF5-0096-7641-98E2-79A7C2A6467A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G39">
     <sortCondition descending="1" ref="E1:E39"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2CA99AFE-1903-6D4B-93D9-DD22E72018C3}" name="Asesor" dataDxfId="53"/>
-    <tableColumn id="8" xr3:uid="{8D0734FC-3769-4F41-9ECD-2C6FE21FFA0E}" name="Clave" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{1247CE0F-8F5E-194F-AD79-C20593AA6B7C}" name="Fecha_Corte" dataDxfId="51"/>
-    <tableColumn id="9" xr3:uid="{1B89683A-64AB-0646-9B15-2B5DA7E1CEEC}" name="Mes_Actual" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{C4F1D3A5-1E56-8C40-9BD7-1C13F22F25C5}" name="PA_Acumulada" dataDxfId="49" dataCellStyle="Millares"/>
-    <tableColumn id="2" xr3:uid="{C05A17F7-6BDD-0C40-A77A-7F7E195BCDDE}" name="Porcentaje_Vida" dataDxfId="48" dataCellStyle="Porcentaje"/>
-    <tableColumn id="5" xr3:uid="{312E2988-4C52-5E40-BB07-41C4565E8822}" name="PA_Faltante_Miembro" dataDxfId="47">
+    <tableColumn id="1" xr3:uid="{2CA99AFE-1903-6D4B-93D9-DD22E72018C3}" name="Asesor" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{8D0734FC-3769-4F41-9ECD-2C6FE21FFA0E}" name="Clave" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{1247CE0F-8F5E-194F-AD79-C20593AA6B7C}" name="Fecha_Corte" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{1B89683A-64AB-0646-9B15-2B5DA7E1CEEC}" name="Mes_Actual" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{C4F1D3A5-1E56-8C40-9BD7-1C13F22F25C5}" name="PA_Acumulada" dataDxfId="8" dataCellStyle="Millares"/>
+    <tableColumn id="2" xr3:uid="{C05A17F7-6BDD-0C40-A77A-7F7E195BCDDE}" name="Porcentaje_Vida" dataDxfId="7" dataCellStyle="Porcentaje"/>
+    <tableColumn id="5" xr3:uid="{312E2988-4C52-5E40-BB07-41C4565E8822}" name="PA_Faltante_Miembro" dataDxfId="6">
       <calculatedColumnFormula>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1975,7 +1272,7 @@
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="12">
         <v>87538</v>
       </c>
       <c r="C2" s="2">
@@ -1987,7 +1284,7 @@
       <c r="E2" s="3">
         <v>4468419.0199999996</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="13">
         <v>1.9914000000000001</v>
       </c>
       <c r="G2" s="8">
@@ -1999,7 +1296,7 @@
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="12">
         <v>80122</v>
       </c>
       <c r="C3" s="2">
@@ -2012,7 +1309,7 @@
       <c r="E3" s="3">
         <v>2062641.64</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="13">
         <v>1.1111</v>
       </c>
       <c r="G3" s="8">
@@ -2024,7 +1321,7 @@
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="12">
         <v>95148</v>
       </c>
       <c r="C4" s="2">
@@ -2037,7 +1334,7 @@
       <c r="E4" s="3">
         <v>1600189.95</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="13">
         <v>0.84589999999999999</v>
       </c>
       <c r="G4" s="8">
@@ -2049,7 +1346,7 @@
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="12">
         <v>47116</v>
       </c>
       <c r="C5" s="2">
@@ -2062,7 +1359,7 @@
       <c r="E5" s="3">
         <v>1499285.01</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="13">
         <v>0.59909999999999997</v>
       </c>
       <c r="G5" s="8">
@@ -2074,7 +1371,7 @@
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>107488</v>
       </c>
       <c r="C6" s="2">
@@ -2087,7 +1384,7 @@
       <c r="E6" s="3">
         <v>1451507.78</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="13">
         <v>0.74990000000000001</v>
       </c>
       <c r="G6" s="8">
@@ -2099,7 +1396,7 @@
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="12">
         <v>110453</v>
       </c>
       <c r="C7" s="2">
@@ -2112,7 +1409,7 @@
       <c r="E7" s="3">
         <v>1272351.1200000001</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="13">
         <v>0.55479999999999996</v>
       </c>
       <c r="G7" s="8">
@@ -2124,7 +1421,7 @@
       <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="12">
         <v>90355</v>
       </c>
       <c r="C8" s="2">
@@ -2137,7 +1434,7 @@
       <c r="E8" s="3">
         <v>1180365.72</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="13">
         <v>0.52900000000000003</v>
       </c>
       <c r="G8" s="8">
@@ -2149,7 +1446,7 @@
       <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="12">
         <v>108404</v>
       </c>
       <c r="C9" s="2">
@@ -2162,7 +1459,7 @@
       <c r="E9" s="3">
         <v>803661.78</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="13">
         <v>0.3755</v>
       </c>
       <c r="G9" s="8">
@@ -2174,7 +1471,7 @@
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="12">
         <v>104718</v>
       </c>
       <c r="C10" s="2">
@@ -2187,7 +1484,7 @@
       <c r="E10" s="3">
         <v>768813.86</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="13">
         <v>0.36220000000000002</v>
       </c>
       <c r="G10" s="8">
@@ -2199,7 +1496,7 @@
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="12">
         <v>108405</v>
       </c>
       <c r="C11" s="2">
@@ -2212,7 +1509,7 @@
       <c r="E11" s="3">
         <v>665005.12</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="13">
         <v>0.3211</v>
       </c>
       <c r="G11" s="8">
@@ -2224,7 +1521,7 @@
       <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>110575</v>
       </c>
       <c r="C12" s="2">
@@ -2237,7 +1534,7 @@
       <c r="E12" s="3">
         <v>626887.43999999994</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="13">
         <v>0.35539999999999999</v>
       </c>
       <c r="G12" s="8">
@@ -2249,7 +1546,7 @@
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <v>105696</v>
       </c>
       <c r="C13" s="2">
@@ -2262,7 +1559,7 @@
       <c r="E13" s="3">
         <v>487715.51</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="13">
         <v>0.20669999999999999</v>
       </c>
       <c r="G13" s="8">
@@ -2274,7 +1571,7 @@
       <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="12">
         <v>104750</v>
       </c>
       <c r="C14" s="2">
@@ -2287,7 +1584,7 @@
       <c r="E14" s="3">
         <v>485147.48</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="13">
         <v>0.22389999999999999</v>
       </c>
       <c r="G14" s="8">
@@ -2299,7 +1596,7 @@
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="12">
         <v>100677</v>
       </c>
       <c r="C15" s="2">
@@ -2312,7 +1609,7 @@
       <c r="E15" s="3">
         <v>484567.65</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="13">
         <v>0.21390000000000001</v>
       </c>
       <c r="G15" s="8">
@@ -2324,7 +1621,7 @@
       <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="12">
         <v>80925</v>
       </c>
       <c r="C16" s="2">
@@ -2337,7 +1634,7 @@
       <c r="E16" s="3">
         <v>477935.47</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="13">
         <v>0.224</v>
       </c>
       <c r="G16" s="8">
@@ -2349,7 +1646,7 @@
       <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="12">
         <v>104343</v>
       </c>
       <c r="C17" s="2">
@@ -2362,7 +1659,7 @@
       <c r="E17" s="3">
         <v>459920.08</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="13">
         <v>0.22989999999999999</v>
       </c>
       <c r="G17" s="8">
@@ -2374,7 +1671,7 @@
       <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="12">
         <v>101640</v>
       </c>
       <c r="C18" s="2">
@@ -2387,7 +1684,7 @@
       <c r="E18" s="3">
         <v>443859.06</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="13">
         <v>0.12280000000000001</v>
       </c>
       <c r="G18" s="8">
@@ -2399,7 +1696,7 @@
       <c r="A19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="12">
         <v>113076</v>
       </c>
       <c r="C19" s="2">
@@ -2412,7 +1709,7 @@
       <c r="E19" s="3">
         <v>384226.53</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="13">
         <v>0.125</v>
       </c>
       <c r="G19" s="8">
@@ -2424,7 +1721,7 @@
       <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="12">
         <v>112083</v>
       </c>
       <c r="C20" s="2">
@@ -2437,7 +1734,7 @@
       <c r="E20" s="3">
         <v>345042.75</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="13">
         <v>0.1069</v>
       </c>
       <c r="G20" s="8">
@@ -2449,7 +1746,7 @@
       <c r="A21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="12">
         <v>113450</v>
       </c>
       <c r="C21" s="2">
@@ -2462,7 +1759,7 @@
       <c r="E21" s="3">
         <v>344516.28</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="13">
         <v>0.13600000000000001</v>
       </c>
       <c r="G21" s="8">
@@ -2474,7 +1771,7 @@
       <c r="A22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="12">
         <v>115047</v>
       </c>
       <c r="C22" s="2">
@@ -2487,7 +1784,7 @@
       <c r="E22" s="3">
         <v>340864.69</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="13">
         <v>0.17230000000000001</v>
       </c>
       <c r="G22" s="8">
@@ -2499,7 +1796,7 @@
       <c r="A23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="12">
         <v>114100</v>
       </c>
       <c r="C23" s="2">
@@ -2512,7 +1809,7 @@
       <c r="E23" s="3">
         <v>313488.28999999998</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="13">
         <v>0.18229999999999999</v>
       </c>
       <c r="G23" s="8">
@@ -2524,7 +1821,7 @@
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="12">
         <v>109998</v>
       </c>
       <c r="C24" s="2">
@@ -2537,7 +1834,7 @@
       <c r="E24" s="3">
         <v>309583.43</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="13">
         <v>0.18</v>
       </c>
       <c r="G24" s="8">
@@ -2549,7 +1846,7 @@
       <c r="A25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="12">
         <v>111960</v>
       </c>
       <c r="C25" s="2">
@@ -2562,7 +1859,7 @@
       <c r="E25" s="3">
         <v>307214.71999999997</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="13">
         <v>0.1724</v>
       </c>
       <c r="G25" s="8">
@@ -2574,7 +1871,7 @@
       <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="12">
         <v>109819</v>
       </c>
       <c r="C26" s="2">
@@ -2587,7 +1884,7 @@
       <c r="E26" s="3">
         <v>251834.49</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="13">
         <v>9.2700000000000005E-2</v>
       </c>
       <c r="G26" s="8">
@@ -2599,7 +1896,7 @@
       <c r="A27" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="12">
         <v>111056</v>
       </c>
       <c r="C27" s="2">
@@ -2612,7 +1909,7 @@
       <c r="E27" s="3">
         <v>246097.69</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="13">
         <v>3.04E-2</v>
       </c>
       <c r="G27" s="8">
@@ -2624,7 +1921,7 @@
       <c r="A28" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="12">
         <v>106018</v>
       </c>
       <c r="C28" s="2">
@@ -2637,7 +1934,7 @@
       <c r="E28" s="3">
         <v>236522.65</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="13">
         <v>0.11899999999999999</v>
       </c>
       <c r="G28" s="8">
@@ -2649,7 +1946,7 @@
       <c r="A29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="12">
         <v>114157</v>
       </c>
       <c r="C29" s="2">
@@ -2662,7 +1959,7 @@
       <c r="E29" s="3">
         <v>205078.7</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="13">
         <v>9.01E-2</v>
       </c>
       <c r="G29" s="8">
@@ -2674,7 +1971,7 @@
       <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="12">
         <v>98797</v>
       </c>
       <c r="C30" s="2">
@@ -2687,7 +1984,7 @@
       <c r="E30" s="3">
         <v>188284.04</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="13">
         <v>6.7400000000000002E-2</v>
       </c>
       <c r="G30" s="8">
@@ -2699,7 +1996,7 @@
       <c r="A31" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="12">
         <v>115404</v>
       </c>
       <c r="C31" s="2">
@@ -2712,7 +2009,7 @@
       <c r="E31" s="3">
         <v>180517.64</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="13">
         <v>9.0700000000000003E-2</v>
       </c>
       <c r="G31" s="8">
@@ -2724,7 +2021,7 @@
       <c r="A32" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="12">
         <v>64502</v>
       </c>
       <c r="C32" s="2">
@@ -2737,7 +2034,7 @@
       <c r="E32" s="3">
         <v>178961.99</v>
       </c>
-      <c r="F32" s="15">
+      <c r="F32" s="13">
         <v>0.10539999999999999</v>
       </c>
       <c r="G32" s="8">
@@ -2749,7 +2046,7 @@
       <c r="A33" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="12">
         <v>112522</v>
       </c>
       <c r="C33" s="2">
@@ -2762,7 +2059,7 @@
       <c r="E33" s="3">
         <v>169406.21</v>
       </c>
-      <c r="F33" s="15">
+      <c r="F33" s="13">
         <v>9.9699999999999997E-2</v>
       </c>
       <c r="G33" s="8">
@@ -2774,7 +2071,7 @@
       <c r="A34" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="12">
         <v>63441</v>
       </c>
       <c r="C34" s="2">
@@ -2787,7 +2084,7 @@
       <c r="E34" s="3">
         <v>164889.29</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="13">
         <v>7.1900000000000006E-2</v>
       </c>
       <c r="G34" s="8">
@@ -2799,7 +2096,7 @@
       <c r="A35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35" s="12">
         <v>109007</v>
       </c>
       <c r="C35" s="2">
@@ -2812,7 +2109,7 @@
       <c r="E35" s="3">
         <v>162789.46</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="13">
         <v>6.2700000000000006E-2</v>
       </c>
       <c r="G35" s="8">
@@ -2824,7 +2121,7 @@
       <c r="A36" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="12">
         <v>114431</v>
       </c>
       <c r="C36" s="2">
@@ -2837,7 +2134,7 @@
       <c r="E36" s="3">
         <v>155492.32999999999</v>
       </c>
-      <c r="F36" s="15">
+      <c r="F36" s="13">
         <v>8.4400000000000003E-2</v>
       </c>
       <c r="G36" s="8">
@@ -2849,7 +2146,7 @@
       <c r="A37" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="12">
         <v>110105</v>
       </c>
       <c r="C37" s="2">
@@ -2862,7 +2159,7 @@
       <c r="E37" s="3">
         <v>153782.96</v>
       </c>
-      <c r="F37" s="15">
+      <c r="F37" s="13">
         <v>9.2799999999999994E-2</v>
       </c>
       <c r="G37" s="8">
@@ -2874,7 +2171,7 @@
       <c r="A38" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="12">
         <v>116060</v>
       </c>
       <c r="C38" s="2">
@@ -2887,7 +2184,7 @@
       <c r="E38" s="4">
         <v>146770.03</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F38" s="13">
         <v>8.6400000000000005E-2</v>
       </c>
       <c r="G38" s="8">
@@ -2899,7 +2196,7 @@
       <c r="A39" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="14">
+      <c r="B39" s="12">
         <v>65046</v>
       </c>
       <c r="C39" s="2">
@@ -2912,7 +2209,7 @@
       <c r="E39" s="4">
         <v>138196.49</v>
       </c>
-      <c r="F39" s="15">
+      <c r="F39" s="13">
         <v>3.6700000000000003E-2</v>
       </c>
       <c r="G39" s="8">
@@ -2924,7 +2221,7 @@
       <c r="A40" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="14">
+      <c r="B40" s="12">
         <v>94205</v>
       </c>
       <c r="C40" s="2">
@@ -2937,7 +2234,7 @@
       <c r="E40" s="4">
         <v>132169.76999999999</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="13">
         <v>6.4399999999999999E-2</v>
       </c>
       <c r="G40" s="8">
@@ -2949,7 +2246,7 @@
       <c r="A41" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="14">
+      <c r="B41" s="12">
         <v>108658</v>
       </c>
       <c r="C41" s="2">
@@ -2962,7 +2259,7 @@
       <c r="E41" s="4">
         <v>114268.52</v>
       </c>
-      <c r="F41" s="15">
+      <c r="F41" s="13">
         <v>5.9200000000000003E-2</v>
       </c>
       <c r="G41" s="8">
@@ -2974,7 +2271,7 @@
       <c r="A42" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="14">
+      <c r="B42" s="12">
         <v>88234</v>
       </c>
       <c r="C42" s="2">
@@ -2987,7 +2284,7 @@
       <c r="E42" s="3">
         <v>96341</v>
       </c>
-      <c r="F42" s="15">
+      <c r="F42" s="13">
         <v>4.1300000000000003E-2</v>
       </c>
       <c r="G42" s="8">
@@ -2999,7 +2296,7 @@
       <c r="A43" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="14">
+      <c r="B43" s="12">
         <v>114664</v>
       </c>
       <c r="C43" s="2">
@@ -3012,7 +2309,7 @@
       <c r="E43" s="10">
         <v>95319.2</v>
       </c>
-      <c r="F43" s="15">
+      <c r="F43" s="13">
         <v>5.6099999999999997E-2</v>
       </c>
       <c r="G43" s="11">
@@ -3021,10 +2318,10 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B44" s="14">
+      <c r="B44" s="12">
         <v>81044</v>
       </c>
       <c r="C44" s="2">
@@ -3037,19 +2334,19 @@
       <c r="E44" s="10">
         <v>94620.24</v>
       </c>
-      <c r="F44" s="15">
+      <c r="F44" s="13">
         <v>-2.5000000000000001E-3</v>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="11">
         <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1603779.76</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="14">
+      <c r="B45" s="12">
         <v>94156</v>
       </c>
       <c r="C45" s="2">
@@ -3062,19 +2359,19 @@
       <c r="E45" s="10">
         <v>54096.08</v>
       </c>
-      <c r="F45" s="15">
+      <c r="F45" s="13">
         <v>2.1299999999999999E-2</v>
       </c>
-      <c r="G45" s="13">
+      <c r="G45" s="11">
         <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1644303.92</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="14">
+      <c r="B46" s="12">
         <v>90177</v>
       </c>
       <c r="C46" s="2">
@@ -3087,19 +2384,19 @@
       <c r="E46" s="10">
         <v>43823.040000000001</v>
       </c>
-      <c r="F46" s="15">
+      <c r="F46" s="13">
         <v>3.5400000000000001E-2</v>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="11">
         <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1654576.96</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="14">
+      <c r="B47" s="12">
         <v>102825</v>
       </c>
       <c r="C47" s="2">
@@ -3112,19 +2409,19 @@
       <c r="E47" s="10">
         <v>38961.82</v>
       </c>
-      <c r="F47" s="15">
+      <c r="F47" s="13">
         <v>2.29E-2</v>
       </c>
-      <c r="G47" s="13">
+      <c r="G47" s="11">
         <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1659438.18</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="12" t="s">
+      <c r="A48" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B48" s="14">
+      <c r="B48" s="12">
         <v>103982</v>
       </c>
       <c r="C48" s="2">
@@ -3137,19 +2434,19 @@
       <c r="E48" s="10">
         <v>28396.89</v>
       </c>
-      <c r="F48" s="15">
+      <c r="F48" s="13">
         <v>0</v>
       </c>
-      <c r="G48" s="13">
+      <c r="G48" s="11">
         <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1670003.11</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="14">
+      <c r="B49" s="12">
         <v>81618</v>
       </c>
       <c r="C49" s="2">
@@ -3162,19 +2459,19 @@
       <c r="E49" s="10">
         <v>9060.02</v>
       </c>
-      <c r="F49" s="15">
+      <c r="F49" s="13">
         <v>5.3E-3</v>
       </c>
-      <c r="G49" s="13">
+      <c r="G49" s="11">
         <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1689339.98</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B50" s="14">
+      <c r="B50" s="12">
         <v>69684</v>
       </c>
       <c r="C50" s="2">
@@ -3187,19 +2484,19 @@
       <c r="E50" s="10">
         <v>1104.3699999999999</v>
       </c>
-      <c r="F50" s="15">
+      <c r="F50" s="13">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="G50" s="13">
+      <c r="G50" s="11">
         <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1697295.63</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="14">
+      <c r="B51" s="12">
         <v>59120</v>
       </c>
       <c r="C51" s="2">
@@ -3212,36 +2509,36 @@
       <c r="E51" s="10">
         <v>0</v>
       </c>
-      <c r="F51" s="15">
+      <c r="F51" s="13">
         <v>0</v>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="11">
         <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1698400</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A51">
-    <cfRule type="expression" dxfId="46" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B51">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+      <formula>$B2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C2:D51">
-    <cfRule type="expression" dxfId="45" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E51">
-    <cfRule type="expression" dxfId="44" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B51">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F51">

</xml_diff>

<commit_message>
Actualizando Meta MDRT 2026 a 1,810,400
</commit_message>
<xml_diff>
--- a/mdrt/mdrt_actual.xlsx
+++ b/mdrt/mdrt_actual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/ ANTIGRAVITY/mdrt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309711E8-8A33-224A-B2FF-6E086CB22681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6913BC-4312-3141-87D2-EB2640F79016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16140" xr2:uid="{B49CA26D-17E4-1041-9F6C-DBD86CE9FF01}"/>
   </bookViews>
@@ -415,6 +415,46 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="6"/>
+        </left>
+        <right style="thin">
+          <color theme="6"/>
+        </right>
+        <top style="thin">
+          <color theme="6"/>
+        </top>
+        <bottom style="thin">
+          <color theme="6"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
@@ -512,46 +552,6 @@
         </top>
         <bottom style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top style="thin">
-          <color theme="6"/>
-        </top>
-        <bottom style="thin">
-          <color theme="6"/>
         </bottom>
       </border>
     </dxf>
@@ -905,8 +905,8 @@
     <tableColumn id="9" xr3:uid="{1B89683A-64AB-0646-9B15-2B5DA7E1CEEC}" name="Mes_Actual" dataDxfId="9"/>
     <tableColumn id="6" xr3:uid="{C4F1D3A5-1E56-8C40-9BD7-1C13F22F25C5}" name="PA_Acumulada" dataDxfId="8" dataCellStyle="Millares"/>
     <tableColumn id="2" xr3:uid="{C05A17F7-6BDD-0C40-A77A-7F7E195BCDDE}" name="Porcentaje_Vida" dataDxfId="7" dataCellStyle="Porcentaje"/>
-    <tableColumn id="5" xr3:uid="{312E2988-4C52-5E40-BB07-41C4565E8822}" name="PA_Faltante_Miembro" dataDxfId="6">
-      <calculatedColumnFormula>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{312E2988-4C52-5E40-BB07-41C4565E8822}" name="PA_Faltante_Miembro" dataDxfId="0">
+      <calculatedColumnFormula>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272306BB-1DE5-9749-A828-31E7777A186B}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1288,8 +1288,8 @@
         <v>1.9914000000000001</v>
       </c>
       <c r="G2" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>-2770019.0199999996</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>-2658019.0199999996</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1313,8 +1313,8 @@
         <v>1.1111</v>
       </c>
       <c r="G3" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>-364241.6399999999</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>-252241.6399999999</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1338,8 +1338,8 @@
         <v>0.84589999999999999</v>
       </c>
       <c r="G4" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>98210.050000000047</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>210210.05000000005</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1363,8 +1363,8 @@
         <v>0.59909999999999997</v>
       </c>
       <c r="G5" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>199114.99</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>311114.99</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1388,8 +1388,8 @@
         <v>0.74990000000000001</v>
       </c>
       <c r="G6" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>246892.21999999997</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>358892.22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1413,8 +1413,8 @@
         <v>0.55479999999999996</v>
       </c>
       <c r="G7" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>426048.87999999989</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>538048.87999999989</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1438,8 +1438,8 @@
         <v>0.52900000000000003</v>
       </c>
       <c r="G8" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>518034.28</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>630034.28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1463,8 +1463,8 @@
         <v>0.3755</v>
       </c>
       <c r="G9" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>894738.22</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1006738.22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1488,8 +1488,8 @@
         <v>0.36220000000000002</v>
       </c>
       <c r="G10" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>929586.14</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1041586.14</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1513,8 +1513,8 @@
         <v>0.3211</v>
       </c>
       <c r="G11" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1033394.88</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1145394.8799999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1538,8 +1538,8 @@
         <v>0.35539999999999999</v>
       </c>
       <c r="G12" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1071512.56</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1183512.56</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1563,8 +1563,8 @@
         <v>0.20669999999999999</v>
       </c>
       <c r="G13" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1210684.49</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1322684.49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1588,8 +1588,8 @@
         <v>0.22389999999999999</v>
       </c>
       <c r="G14" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1213252.52</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1325252.52</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1613,8 +1613,8 @@
         <v>0.21390000000000001</v>
       </c>
       <c r="G15" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1213832.3500000001</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1325832.3500000001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1638,8 +1638,8 @@
         <v>0.224</v>
       </c>
       <c r="G16" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1220464.53</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1332464.53</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1663,8 +1663,8 @@
         <v>0.22989999999999999</v>
       </c>
       <c r="G17" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1238479.92</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1350479.92</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1688,8 +1688,8 @@
         <v>0.12280000000000001</v>
       </c>
       <c r="G18" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1254540.94</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1366540.94</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1713,8 +1713,8 @@
         <v>0.125</v>
       </c>
       <c r="G19" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1314173.47</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1426173.47</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1738,8 +1738,8 @@
         <v>0.1069</v>
       </c>
       <c r="G20" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1353357.25</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1465357.25</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1763,8 +1763,8 @@
         <v>0.13600000000000001</v>
       </c>
       <c r="G21" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1353883.72</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1465883.72</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1788,8 +1788,8 @@
         <v>0.17230000000000001</v>
       </c>
       <c r="G22" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1357535.31</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1469535.31</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1813,8 +1813,8 @@
         <v>0.18229999999999999</v>
       </c>
       <c r="G23" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1384911.71</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1496911.71</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1838,8 +1838,8 @@
         <v>0.18</v>
       </c>
       <c r="G24" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1388816.57</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1500816.57</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1863,8 +1863,8 @@
         <v>0.1724</v>
       </c>
       <c r="G25" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1391185.28</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1503185.28</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1888,8 +1888,8 @@
         <v>9.2700000000000005E-2</v>
       </c>
       <c r="G26" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1446565.51</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1558565.51</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1913,8 +1913,8 @@
         <v>3.04E-2</v>
       </c>
       <c r="G27" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1452302.31</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1564302.31</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1938,8 +1938,8 @@
         <v>0.11899999999999999</v>
       </c>
       <c r="G28" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1461877.35</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1573877.35</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1963,8 +1963,8 @@
         <v>9.01E-2</v>
       </c>
       <c r="G29" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1493321.3</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1605321.3</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1988,8 +1988,8 @@
         <v>6.7400000000000002E-2</v>
       </c>
       <c r="G30" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1510115.96</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1622115.96</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -2013,8 +2013,8 @@
         <v>9.0700000000000003E-2</v>
       </c>
       <c r="G31" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1517882.3599999999</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1629882.3599999999</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -2038,8 +2038,8 @@
         <v>0.10539999999999999</v>
       </c>
       <c r="G32" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1519438.01</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1631438.01</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -2063,8 +2063,8 @@
         <v>9.9699999999999997E-2</v>
       </c>
       <c r="G33" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1528993.79</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1640993.79</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -2088,8 +2088,8 @@
         <v>7.1900000000000006E-2</v>
       </c>
       <c r="G34" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1533510.71</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1645510.71</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -2113,8 +2113,8 @@
         <v>6.2700000000000006E-2</v>
       </c>
       <c r="G35" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1535610.54</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1647610.54</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -2138,8 +2138,8 @@
         <v>8.4400000000000003E-2</v>
       </c>
       <c r="G36" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1542907.67</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1654907.67</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -2163,8 +2163,8 @@
         <v>9.2799999999999994E-2</v>
       </c>
       <c r="G37" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1544617.04</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1656617.04</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -2188,8 +2188,8 @@
         <v>8.6400000000000005E-2</v>
       </c>
       <c r="G38" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1551629.97</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1663629.97</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -2213,8 +2213,8 @@
         <v>3.6700000000000003E-2</v>
       </c>
       <c r="G39" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1560203.51</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1672203.51</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2238,8 +2238,8 @@
         <v>6.4399999999999999E-2</v>
       </c>
       <c r="G40" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1566230.23</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1678230.23</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -2263,8 +2263,8 @@
         <v>5.9200000000000003E-2</v>
       </c>
       <c r="G41" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1584131.48</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1696131.48</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -2288,8 +2288,8 @@
         <v>4.1300000000000003E-2</v>
       </c>
       <c r="G42" s="8">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1602059</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1714059</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -2313,8 +2313,8 @@
         <v>5.6099999999999997E-2</v>
       </c>
       <c r="G43" s="11">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1603080.8</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1715080.8</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -2338,8 +2338,8 @@
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="G44" s="11">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1603779.76</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1715779.76</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -2363,8 +2363,8 @@
         <v>2.1299999999999999E-2</v>
       </c>
       <c r="G45" s="11">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1644303.92</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1756303.92</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -2388,8 +2388,8 @@
         <v>3.5400000000000001E-2</v>
       </c>
       <c r="G46" s="11">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1654576.96</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1766576.96</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -2413,8 +2413,8 @@
         <v>2.29E-2</v>
       </c>
       <c r="G47" s="11">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1659438.18</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1771438.18</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2438,8 +2438,8 @@
         <v>0</v>
       </c>
       <c r="G48" s="11">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1670003.11</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1782003.11</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -2463,8 +2463,8 @@
         <v>5.3E-3</v>
       </c>
       <c r="G49" s="11">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1689339.98</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1801339.98</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -2488,8 +2488,8 @@
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="G50" s="11">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1697295.63</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1809295.63</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -2513,36 +2513,36 @@
         <v>0</v>
       </c>
       <c r="G51" s="11">
-        <f>(1698400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
-        <v>1698400</v>
+        <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>1810400</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A51">
-    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B51">
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:D51">
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E51">
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F51">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Lanzamiento Triple Corona MDRT: Member, COT y TOT
</commit_message>
<xml_diff>
--- a/mdrt/mdrt_actual.xlsx
+++ b/mdrt/mdrt_actual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/ ANTIGRAVITY/mdrt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499A9365-2DB4-4A4E-AD00-B73E2742296B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F372BD2C-8A15-CC4E-8155-96FB3D1A65C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16140" xr2:uid="{B49CA26D-17E4-1041-9F6C-DBD86CE9FF01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>MONICA ANDREA AMBRIZ GOMEZ</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>LINDA TANIA MIROSLAVA ENRIQUEZ PRECIADO</t>
+  </si>
+  <si>
+    <t>PA_Faltante_COT</t>
+  </si>
+  <si>
+    <t>PA_Faltante_TOT</t>
   </si>
 </sst>
 </file>
@@ -270,7 +276,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -358,13 +364,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF505050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF505050"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF505050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -407,29 +426,26 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="20">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
       </font>
       <numFmt numFmtId="3" formatCode="#,##0"/>
       <fill>
@@ -438,21 +454,23 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top style="thin">
-          <color theme="6"/>
-        </top>
-        <bottom style="thin">
-          <color theme="6"/>
-        </bottom>
-      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -552,6 +570,46 @@
         </top>
         <bottom style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="6"/>
+        </left>
+        <right style="thin">
+          <color theme="6"/>
+        </right>
+        <top style="thin">
+          <color theme="6"/>
+        </top>
+        <bottom style="thin">
+          <color theme="6"/>
         </bottom>
       </border>
     </dxf>
@@ -893,20 +951,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E315FDF5-0096-7641-98E2-79A7C2A6467A}" name="Tabla1354" displayName="Tabla1354" ref="A1:G51" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="A1:G51" xr:uid="{E315FDF5-0096-7641-98E2-79A7C2A6467A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E315FDF5-0096-7641-98E2-79A7C2A6467A}" name="Tabla1354" displayName="Tabla1354" ref="A1:I51" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="A1:I51" xr:uid="{E315FDF5-0096-7641-98E2-79A7C2A6467A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G39">
     <sortCondition descending="1" ref="E1:E39"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2CA99AFE-1903-6D4B-93D9-DD22E72018C3}" name="Asesor" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{8D0734FC-3769-4F41-9ECD-2C6FE21FFA0E}" name="Clave" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{1247CE0F-8F5E-194F-AD79-C20593AA6B7C}" name="Fecha_Corte" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{1B89683A-64AB-0646-9B15-2B5DA7E1CEEC}" name="Mes_Actual" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{C4F1D3A5-1E56-8C40-9BD7-1C13F22F25C5}" name="PA_Acumulada" dataDxfId="8" dataCellStyle="Millares"/>
-    <tableColumn id="2" xr3:uid="{C05A17F7-6BDD-0C40-A77A-7F7E195BCDDE}" name="Porcentaje_Vida" dataDxfId="7" dataCellStyle="Porcentaje"/>
-    <tableColumn id="5" xr3:uid="{312E2988-4C52-5E40-BB07-41C4565E8822}" name="PA_Faltante_Miembro" dataDxfId="0">
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{2CA99AFE-1903-6D4B-93D9-DD22E72018C3}" name="Asesor" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{8D0734FC-3769-4F41-9ECD-2C6FE21FFA0E}" name="Clave" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{1247CE0F-8F5E-194F-AD79-C20593AA6B7C}" name="Fecha_Corte" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{1B89683A-64AB-0646-9B15-2B5DA7E1CEEC}" name="Mes_Actual" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{C4F1D3A5-1E56-8C40-9BD7-1C13F22F25C5}" name="PA_Acumulada" dataDxfId="10" dataCellStyle="Millares"/>
+    <tableColumn id="2" xr3:uid="{C05A17F7-6BDD-0C40-A77A-7F7E195BCDDE}" name="Porcentaje_Vida" dataDxfId="9" dataCellStyle="Porcentaje"/>
+    <tableColumn id="5" xr3:uid="{312E2988-4C52-5E40-BB07-41C4565E8822}" name="PA_Faltante_Miembro" dataDxfId="8">
       <calculatedColumnFormula>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{23B4CB44-7ED7-6447-B4E6-57750E16FB9F}" name="PA_Faltante_COT" dataDxfId="1">
+      <calculatedColumnFormula>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{679BA0C2-1B45-3B41-B8E0-2A7F06B81728}" name="PA_Faltante_TOT" dataDxfId="0">
+      <calculatedColumnFormula>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1230,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272306BB-1DE5-9749-A828-31E7777A186B}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1245,7 +1309,7 @@
     <col min="7" max="7" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>39</v>
       </c>
@@ -1267,8 +1331,14 @@
       <c r="G1" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1291,8 +1361,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>-2658019.0199999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>962780.98000000045</v>
+      </c>
+      <c r="I2" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>6393980.9800000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1316,8 +1394,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>-252241.6399999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>3368558.3600000003</v>
+      </c>
+      <c r="I3" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>8799758.3599999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
@@ -1341,8 +1427,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>210210.05000000005</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>3831010.05</v>
+      </c>
+      <c r="I4" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>9262210.0500000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1366,8 +1460,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>311114.99</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>3931914.99</v>
+      </c>
+      <c r="I5" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>9363114.9900000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -1391,8 +1493,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>358892.22</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>3979692.2199999997</v>
+      </c>
+      <c r="I6" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>9410892.2200000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1416,8 +1526,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>538048.87999999989</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4158848.88</v>
+      </c>
+      <c r="I7" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>9590048.879999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
@@ -1441,8 +1559,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>630034.28</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4250834.28</v>
+      </c>
+      <c r="I8" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>9682034.2799999993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
@@ -1466,8 +1592,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1006738.22</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4627538.22</v>
+      </c>
+      <c r="I9" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10058738.220000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
@@ -1491,8 +1625,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1041586.14</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4662386.1399999997</v>
+      </c>
+      <c r="I10" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10093586.140000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
@@ -1516,8 +1658,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1145394.8799999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4766194.88</v>
+      </c>
+      <c r="I11" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10197394.880000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
@@ -1541,8 +1691,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1183512.56</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4804312.5600000005</v>
+      </c>
+      <c r="I12" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10235512.560000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -1566,8 +1724,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1322684.49</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4943484.49</v>
+      </c>
+      <c r="I13" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10374684.49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
@@ -1591,8 +1757,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1325252.52</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4946052.5199999996</v>
+      </c>
+      <c r="I14" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10377252.52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1616,8 +1790,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1325832.3500000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4946632.3499999996</v>
+      </c>
+      <c r="I15" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10377832.35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
@@ -1641,8 +1823,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1332464.53</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4953264.53</v>
+      </c>
+      <c r="I16" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10384464.529999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
@@ -1666,8 +1856,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1350479.92</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4971279.92</v>
+      </c>
+      <c r="I17" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10402479.92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
@@ -1691,8 +1889,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1366540.94</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>4987340.9400000004</v>
+      </c>
+      <c r="I18" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10418540.939999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>47</v>
       </c>
@@ -1716,8 +1922,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1426173.47</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5046973.47</v>
+      </c>
+      <c r="I19" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10478173.470000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
@@ -1741,8 +1955,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1465357.25</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5086157.25</v>
+      </c>
+      <c r="I20" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10517357.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>46</v>
       </c>
@@ -1766,8 +1988,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1465883.72</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5086683.72</v>
+      </c>
+      <c r="I21" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10517883.720000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>48</v>
       </c>
@@ -1791,8 +2021,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1469535.31</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5090335.3099999996</v>
+      </c>
+      <c r="I22" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10521535.310000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>49</v>
       </c>
@@ -1816,8 +2054,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1496911.71</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5117711.71</v>
+      </c>
+      <c r="I23" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10548911.710000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
@@ -1841,8 +2087,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1500816.57</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5121616.57</v>
+      </c>
+      <c r="I24" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10552816.57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>6</v>
       </c>
@@ -1866,8 +2120,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1503185.28</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5123985.28</v>
+      </c>
+      <c r="I25" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10555185.279999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
@@ -1891,8 +2153,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1558565.51</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5179365.51</v>
+      </c>
+      <c r="I26" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10610565.51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>22</v>
       </c>
@@ -1916,8 +2186,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1564302.31</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5185102.3099999996</v>
+      </c>
+      <c r="I27" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10616302.310000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>15</v>
       </c>
@@ -1941,8 +2219,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1573877.35</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5194677.3499999996</v>
+      </c>
+      <c r="I28" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10625877.35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>50</v>
       </c>
@@ -1966,8 +2252,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1605321.3</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5226121.3</v>
+      </c>
+      <c r="I29" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10657321.300000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
@@ -1991,8 +2285,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1622115.96</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5242915.96</v>
+      </c>
+      <c r="I30" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10674115.960000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>51</v>
       </c>
@@ -2016,8 +2318,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1629882.3599999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5250682.3600000003</v>
+      </c>
+      <c r="I31" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10681882.359999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>31</v>
       </c>
@@ -2041,8 +2351,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1631438.01</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5252238.01</v>
+      </c>
+      <c r="I32" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10683438.01</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>52</v>
       </c>
@@ -2066,8 +2384,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1640993.79</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5261793.79</v>
+      </c>
+      <c r="I33" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10692993.789999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>23</v>
       </c>
@@ -2091,8 +2417,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1645510.71</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5266310.71</v>
+      </c>
+      <c r="I34" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10697510.710000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>21</v>
       </c>
@@ -2116,8 +2450,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1647610.54</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5268410.54</v>
+      </c>
+      <c r="I35" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10699610.539999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>53</v>
       </c>
@@ -2141,8 +2483,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1654907.67</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5275707.67</v>
+      </c>
+      <c r="I36" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10706907.67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>25</v>
       </c>
@@ -2166,8 +2516,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1656617.04</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5277417.04</v>
+      </c>
+      <c r="I37" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10708617.039999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>54</v>
       </c>
@@ -2191,8 +2549,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1663629.97</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5284429.97</v>
+      </c>
+      <c r="I38" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10715629.970000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>27</v>
       </c>
@@ -2216,8 +2582,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1672203.51</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5293003.51</v>
+      </c>
+      <c r="I39" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10724203.51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>55</v>
       </c>
@@ -2241,8 +2615,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1678230.23</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5299030.2300000004</v>
+      </c>
+      <c r="I40" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10730230.23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>17</v>
       </c>
@@ -2266,8 +2648,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1696131.48</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5316931.4800000004</v>
+      </c>
+      <c r="I41" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10748131.48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>24</v>
       </c>
@@ -2291,8 +2681,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1714059</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" s="14">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5334859</v>
+      </c>
+      <c r="I42" s="14">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10766059</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>56</v>
       </c>
@@ -2316,8 +2714,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1715080.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" s="15">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5335880.8</v>
+      </c>
+      <c r="I43" s="15">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10767080.800000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>26</v>
       </c>
@@ -2341,8 +2747,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1715779.76</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44" s="15">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5336579.76</v>
+      </c>
+      <c r="I44" s="15">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10767779.76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>29</v>
       </c>
@@ -2366,8 +2780,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1756303.92</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" s="15">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5377103.9199999999</v>
+      </c>
+      <c r="I45" s="15">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10808303.92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>38</v>
       </c>
@@ -2391,8 +2813,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1766576.96</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" s="15">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5387376.96</v>
+      </c>
+      <c r="I46" s="15">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10818576.960000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>33</v>
       </c>
@@ -2416,8 +2846,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1771438.18</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" s="15">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5392238.1799999997</v>
+      </c>
+      <c r="I47" s="15">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10823438.18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>35</v>
       </c>
@@ -2441,8 +2879,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1782003.11</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="15">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5402803.1100000003</v>
+      </c>
+      <c r="I48" s="15">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10834003.109999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>36</v>
       </c>
@@ -2466,8 +2912,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1801339.98</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" s="15">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5422139.9800000004</v>
+      </c>
+      <c r="I49" s="15">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10853339.98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>32</v>
       </c>
@@ -2491,8 +2945,16 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1809295.63</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="15">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5430095.6299999999</v>
+      </c>
+      <c r="I50" s="15">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10861295.630000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>37</v>
       </c>
@@ -2516,33 +2978,41 @@
         <f>(1810400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
         <v>1810400</v>
       </c>
+      <c r="H51" s="15">
+        <f>(5431200-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>5431200</v>
+      </c>
+      <c r="I51" s="15">
+        <f>(10862400-Tabla1354[[#This Row],[PA_Acumulada]])</f>
+        <v>10862400</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A51">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B51">
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:D51">
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E51">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F51">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>